<commit_message>
ACDynamicStabilityManager, first complete calculation test, with aero data read from file. Under development!
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON_CANARD_LOOP2_DYN/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/IRON_CANARD_LOOP2_DYN/BALANCE/Balance.xlsx
@@ -258,10 +258,10 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
-  </si>
-  <si>
-    <t>TORENBEEK_1982</t>
   </si>
   <si>
     <t>Ycg LRF (semi-wing)</t>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -1876,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>15.527255597045638</v>
+        <v>17.878799999999995</v>
       </c>
     </row>
     <row r="24">
@@ -1887,7 +1887,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>17.878799999999995</v>
+        <v>15.527255597045638</v>
       </c>
     </row>
   </sheetData>
@@ -2127,7 +2127,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>2.2926530320804064</v>
+        <v>1.8563139127409203</v>
       </c>
     </row>
     <row r="24">
@@ -2138,7 +2138,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>1.8563139127409203</v>
+        <v>2.2926530320804064</v>
       </c>
     </row>
     <row r="25">
@@ -2159,7 +2159,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>7.957351173907407</v>
+        <v>6.868233768733532</v>
       </c>
     </row>
     <row r="28">
@@ -2170,7 +2170,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>6.868233768733532</v>
+        <v>7.957351173907407</v>
       </c>
     </row>
   </sheetData>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2649,7 +2649,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>

</xml_diff>